<commit_message>
Added event to test.xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitrapeddireddy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitrapeddireddy/Documents/GitHub/lfp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4C496B8-CB1E-A145-8F83-2491A1F03512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA6712E-C963-2A49-A464-D7A8196453A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2FAFBB3C-B1F6-3A4E-ACAC-DAC127624BD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="30">
   <si>
     <t>time</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>omission</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>win</t>
   </si>
 </sst>
 </file>
@@ -475,15 +484,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1954181E-5C73-8142-A2BE-690E990E3CDF}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="63.1640625" customWidth="1"/>
+    <col min="5" max="5" width="72.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" customWidth="1"/>
+    <col min="11" max="11" width="38.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -518,10 +535,13 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1843</v>
       </c>
@@ -559,11 +579,14 @@
         <v>1.4</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1844</v>
       </c>
@@ -601,11 +624,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1845</v>
       </c>
@@ -643,11 +669,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1846</v>
       </c>
@@ -685,11 +714,14 @@
         <v>1.4</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1847</v>
       </c>
@@ -727,11 +759,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1848</v>
       </c>
@@ -769,11 +804,14 @@
         <v>1.4</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1849</v>
       </c>
@@ -811,11 +849,14 @@
         <v>1.4</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1850</v>
       </c>
@@ -853,11 +894,14 @@
         <v>1.4</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1851</v>
       </c>
@@ -895,11 +939,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1852</v>
       </c>
@@ -937,13 +984,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1853</v>
       </c>
@@ -981,11 +1031,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1854</v>
       </c>
@@ -1023,11 +1076,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1855</v>
       </c>
@@ -1065,11 +1121,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1856</v>
       </c>
@@ -1107,11 +1166,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1857</v>
       </c>
@@ -1149,11 +1211,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1858</v>
       </c>
@@ -1191,13 +1256,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1859</v>
       </c>
@@ -1235,11 +1303,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1860</v>
       </c>
@@ -1277,11 +1348,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1861</v>
       </c>
@@ -1319,11 +1393,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1862</v>
       </c>
@@ -1361,11 +1438,14 @@
         <v>1.4</v>
       </c>
       <c r="M21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1863</v>
       </c>
@@ -1402,10 +1482,13 @@
       <c r="L22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1864</v>
       </c>
@@ -1442,10 +1525,13 @@
       <c r="L23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1865</v>
       </c>
@@ -1482,10 +1568,13 @@
       <c r="L24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1866</v>
       </c>
@@ -1522,10 +1611,13 @@
       <c r="L25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1867</v>
       </c>
@@ -1562,10 +1654,13 @@
       <c r="L26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="1"/>
+      <c r="M26" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1868</v>
       </c>
@@ -1602,10 +1697,13 @@
       <c r="L27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="1"/>
+      <c r="M27" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1869</v>
       </c>
@@ -1642,10 +1740,13 @@
       <c r="L28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1870</v>
       </c>
@@ -1682,10 +1783,13 @@
       <c r="L29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1871</v>
       </c>
@@ -1722,10 +1826,13 @@
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1872</v>
       </c>
@@ -1762,10 +1869,13 @@
       <c r="L31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1873</v>
       </c>
@@ -1802,10 +1912,13 @@
       <c r="L32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1874</v>
       </c>
@@ -1842,10 +1955,13 @@
       <c r="L33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1875</v>
       </c>
@@ -1882,10 +1998,13 @@
       <c r="L34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1876</v>
       </c>
@@ -1922,10 +2041,13 @@
       <c r="L35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1877</v>
       </c>
@@ -1962,10 +2084,13 @@
       <c r="L36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>1878</v>
       </c>
@@ -2002,10 +2127,13 @@
       <c r="L37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1879</v>
       </c>
@@ -2042,10 +2170,13 @@
       <c r="L38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M38" s="1"/>
+      <c r="M38" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1880</v>
       </c>
@@ -2082,12 +2213,15 @@
       <c r="L39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="1"/>
+      <c r="M39" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M39" xr:uid="{0CC0220A-3FBF-0E4A-A923-E06BAE1BB4F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N39" xr:uid="{0CC0220A-3FBF-0E4A-A923-E06BAE1BB4F8}">
       <formula1>"Subj 1 Only,Subj 2 Only,Close Call,Subj 1 then Subj 2,Subj 2 then Subj 1,Subj 1 blocking Subj 2,Subj 2 blocking Subj 1"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added notes from mtg 12/13
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitrapeddireddy/Documents/GitHub/lfp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883BD340-4B85-1842-94FF-69320BB01D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DEC8B5-AEAE-A747-BC45-6C94183A1D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{2FAFBB3C-B1F6-3A4E-ACAC-DAC127624BD3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2FAFBB3C-B1F6-3A4E-ACAC-DAC127624BD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1954181E-5C73-8142-A2BE-690E990E3CDF}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,8 +561,8 @@
         <v>1934930</v>
       </c>
       <c r="C2" s="1">
-        <f>B2+10000</f>
-        <v>1944930</v>
+        <f>B2+200000</f>
+        <v>2134930</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -613,8 +613,8 @@
         <v>4334936</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C39" si="0">B3+10000</f>
-        <v>4344936</v>
+        <f t="shared" ref="C3:C39" si="0">B3+200000</f>
+        <v>4534936</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -666,7 +666,7 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>6644931</v>
+        <v>6834931</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -718,7 +718,7 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>8444930</v>
+        <v>8634930</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -770,7 +770,7 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>9544930</v>
+        <v>9734930</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>10544929</v>
+        <v>10734929</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -874,7 +874,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>12444926</v>
+        <v>12634926</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -926,7 +926,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>13944925</v>
+        <v>14134925</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -978,7 +978,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>16044924</v>
+        <v>16234924</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>17044926</v>
+        <v>17234926</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>18644925</v>
+        <v>18834925</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>19944925</v>
+        <v>20134925</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>21244922</v>
+        <v>21434922</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>22244924</v>
+        <v>22434924</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>23644923</v>
+        <v>23834923</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>25544923</v>
+        <v>25734923</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>27144920</v>
+        <v>27334920</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>28544922</v>
+        <v>28734922</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>30744921</v>
+        <v>30934921</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>31944918</v>
+        <v>32134918</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>37944919</v>
+        <v>38134919</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>39144916</v>
+        <v>39334916</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>40244916</v>
+        <v>40434916</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>41544918</v>
+        <v>41734918</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
-        <v>42644918</v>
+        <v>42834918</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>43644915</v>
+        <v>43834915</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
-        <v>44644917</v>
+        <v>44834917</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
-        <v>46744914</v>
+        <v>46934914</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
-        <v>49144915</v>
+        <v>49334915</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
-        <v>51544912</v>
+        <v>51734912</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
-        <v>53744914</v>
+        <v>53934914</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
-        <v>55444913</v>
+        <v>55634913</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
-        <v>57844912</v>
+        <v>58034912</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -2256,7 +2256,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
-        <v>59044912</v>
+        <v>59234912</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
-        <v>60344909</v>
+        <v>60534909</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
-        <v>61544911</v>
+        <v>61734911</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
-        <v>63044911</v>
+        <v>63234911</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="0"/>
-        <v>65044907</v>
+        <v>65234907</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>

</xml_diff>